<commit_message>
Atualizacoes finais - Sistema AbsenteismoController v2.0 funcionando
</commit_message>
<xml_diff>
--- a/Dados/INDICADORES SETEMBRO 2025.xlsx
+++ b/Dados/INDICADORES SETEMBRO 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CONVER\INDICADORES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ede Machado\AbsenteismoController\Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D95DA9-EE40-4881-84CF-A935FBA601AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42250EB-BE29-4900-80EC-1AE5E82302DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{FE1881E6-0893-49A4-AF32-F06F2506CEDE}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{FE1881E6-0893-49A4-AF32-F06F2506CEDE}"/>
   </bookViews>
   <sheets>
     <sheet name="NÚMERO DE ATESTADOS" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -4793,14 +4804,10 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4838,7 +4845,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4944,7 +4951,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5086,7 +5093,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5097,7 +5104,7 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:S32"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>